<commit_message>
add new test.xl, add 시트1,시트2,시트3 buttons
</commit_message>
<xml_diff>
--- a/excelhere/room_five.xlsx
+++ b/excelhere/room_five.xlsx
@@ -444,17 +444,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>0005</t>
+          <t>000001</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>하경택</t>
+          <t>hong</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>성승헌</t>
+          <t>gil</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -506,7 +506,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>접시100</t>
+          <t>노트</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -515,19 +515,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>닭볶음탕</t>
+          <t>육개장(컵)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -536,19 +536,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9000</v>
+        <v>1050</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>9000</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>양념치킨</t>
+          <t>접시100</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -557,19 +557,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9000</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>9000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>콜라</t>
+          <t>육개장(컵)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>1050</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>1000</v>
+        <v>1050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>